<commit_message>
Updated cao 10:07am, 20 August 2014.
</commit_message>
<xml_diff>
--- a/Team FOL Scheduling.xlsx
+++ b/Team FOL Scheduling.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
   <si>
     <t>Days</t>
   </si>
@@ -197,7 +197,46 @@
     <t>Tasks/Duration(Days)</t>
   </si>
   <si>
-    <t>Note: First Monday is not included in this schedule as it was done to do all the planning.</t>
+    <t>Wei Heng</t>
+  </si>
+  <si>
+    <t>B&amp;T</t>
+  </si>
+  <si>
+    <t>T&amp;W</t>
+  </si>
+  <si>
+    <t>B&amp;T&amp;W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: </t>
+  </si>
+  <si>
+    <t>B = Brandon</t>
+  </si>
+  <si>
+    <t>T = Troy</t>
+  </si>
+  <si>
+    <t>W = Wei Heng</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>First Monday is not included</t>
+  </si>
+  <si>
+    <t>Link the menu with game</t>
+  </si>
+  <si>
+    <t>Play Test &amp; Ensure game is fluid</t>
+  </si>
+  <si>
+    <t>Reserved for last minute changes</t>
   </si>
 </sst>
 </file>
@@ -228,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,8 +328,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -314,19 +377,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -341,244 +391,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -612,79 +429,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1206,19 +985,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U39"/>
+  <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
     <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.88671875" customWidth="1"/>
     <col min="10" max="10" width="16.109375" customWidth="1"/>
     <col min="11" max="11" width="16.44140625" customWidth="1"/>
@@ -1573,49 +1354,49 @@
       <c r="U24" s="5"/>
     </row>
     <row r="25" spans="1:21" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="45" t="s">
+      <c r="F25" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="52" t="s">
+      <c r="G25" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="48" t="s">
+      <c r="H25" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I25" s="20" t="s">
+      <c r="I25" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J25" s="20" t="s">
+      <c r="J25" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="K25" s="20" t="s">
+      <c r="K25" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L25" s="20" t="s">
+      <c r="L25" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="M25" s="20" t="s">
+      <c r="M25" s="13" t="s">
         <v>8</v>
       </c>
       <c r="N25" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="O25" s="55" t="s">
+      <c r="O25" s="31" t="s">
         <v>10</v>
       </c>
       <c r="P25" s="5"/>
@@ -1625,59 +1406,59 @@
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
     </row>
-    <row r="26" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="27" t="s">
+    <row r="26" spans="1:21" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="62" t="s">
+      <c r="B26" s="14"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="H26" s="49"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="39"/>
-      <c r="N26" s="42" t="s">
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="O26" s="56" t="s">
+      <c r="O26" s="31" t="s">
         <v>45</v>
       </c>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
       <c r="S26" s="5"/>
-      <c r="T26" s="66"/>
+      <c r="T26" s="20"/>
       <c r="U26" s="5"/>
     </row>
-    <row r="27" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="28" t="s">
+    <row r="27" spans="1:21" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="63" t="s">
+      <c r="B27" s="14"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="H27" s="26"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="43" t="s">
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="O27" s="57" t="s">
+      <c r="O27" s="31" t="s">
         <v>49</v>
       </c>
       <c r="P27" s="5"/>
@@ -1687,30 +1468,30 @@
       <c r="T27" s="5"/>
       <c r="U27" s="5"/>
     </row>
-    <row r="28" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="28" t="s">
+    <row r="28" spans="1:21" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="65" t="s">
+      <c r="B28" s="16"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="63" t="s">
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="H28" s="26"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="43" t="s">
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="O28" s="61" t="s">
+      <c r="O28" s="34" t="s">
         <v>54</v>
       </c>
       <c r="P28" s="7"/>
@@ -1720,59 +1501,59 @@
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
     </row>
-    <row r="29" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="28" t="s">
+    <row r="29" spans="1:21" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="63" t="s">
+      <c r="B29" s="16"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="H29" s="26"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="43" t="s">
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="O29" s="61" t="s">
+      <c r="O29" s="34" t="s">
         <v>49</v>
       </c>
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
       <c r="S29" s="5"/>
-      <c r="T29" s="66"/>
+      <c r="T29" s="20"/>
       <c r="U29" s="5"/>
     </row>
-    <row r="30" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="28" t="s">
+    <row r="30" spans="1:21" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="63" t="s">
+      <c r="B30" s="15"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="H30" s="26"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="40"/>
-      <c r="N30" s="43" t="s">
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="O30" s="61" t="s">
+      <c r="O30" s="34" t="s">
         <v>55</v>
       </c>
       <c r="P30" s="5"/>
@@ -1782,28 +1563,34 @@
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
     </row>
-    <row r="31" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="28" t="s">
+    <row r="31" spans="1:21" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="16" t="s">
+      <c r="B31" s="13"/>
+      <c r="C31" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="40"/>
-      <c r="N31" s="43" t="s">
+      <c r="D31" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="17"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="O31" s="61" t="s">
+      <c r="O31" s="34" t="s">
         <v>45</v>
       </c>
       <c r="P31" s="7"/>
@@ -1813,51 +1600,53 @@
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
     </row>
-    <row r="32" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="28" t="s">
+    <row r="32" spans="1:21" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="40"/>
-      <c r="N32" s="43" t="s">
+      <c r="B32" s="13"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="O32" s="57"/>
+      <c r="O32" s="31"/>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
-      <c r="T32" s="66"/>
+      <c r="T32" s="20"/>
       <c r="U32" s="5"/>
     </row>
-    <row r="33" spans="1:21" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="41"/>
-      <c r="N33" s="44"/>
-      <c r="O33" s="58"/>
+    <row r="33" spans="1:21" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="29"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
@@ -1865,8 +1654,24 @@
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
     </row>
-    <row r="34" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D34" s="1"/>
+    <row r="34" spans="1:21" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="31"/>
       <c r="P34" s="7"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
@@ -1875,19 +1680,16 @@
       <c r="U34" s="1"/>
     </row>
     <row r="35" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="60" t="s">
+      <c r="C35" s="19" t="s">
         <v>52</v>
       </c>
       <c r="D35" s="1"/>
-      <c r="E35" s="59" t="s">
-        <v>57</v>
-      </c>
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
       <c r="R35" s="5"/>
@@ -1896,42 +1698,95 @@
       <c r="U35" s="5"/>
     </row>
     <row r="36" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="32"/>
-      <c r="C36" s="31">
+      <c r="B36" s="14"/>
+      <c r="C36" s="13">
         <v>92232298</v>
       </c>
       <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="33"/>
-      <c r="C37" s="31">
+      <c r="B37" s="15"/>
+      <c r="C37" s="13">
         <v>91381285</v>
       </c>
       <c r="D37" s="1"/>
+      <c r="E37" s="19" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="38" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="34"/>
-      <c r="C38" s="31">
+      <c r="B38" s="16"/>
+      <c r="C38" s="13">
         <v>81119746</v>
       </c>
+      <c r="E38" s="13" t="s">
+        <v>67</v>
+      </c>
       <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="23"/>
+      <c r="C39" s="13">
+        <v>97113472</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="26"/>
+      <c r="C40" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="22"/>
+      <c r="C41" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="29"/>
+      <c r="C42" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="35"/>
-      <c r="C39" s="31"/>
-      <c r="F39" s="11"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="25" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes made to the presentation slides.
</commit_message>
<xml_diff>
--- a/Team FOL Scheduling.xlsx
+++ b/Team FOL Scheduling.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
   <si>
     <t>Days</t>
   </si>
@@ -164,33 +164,15 @@
     <t>Presentation</t>
   </si>
   <si>
-    <t>Preparations</t>
-  </si>
-  <si>
-    <t>And</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
     <t>Day</t>
   </si>
   <si>
     <t>Program Menu/AI</t>
   </si>
   <si>
-    <t>Check by Brandon</t>
-  </si>
-  <si>
     <t>Contact Number</t>
   </si>
   <si>
-    <t>Initial Compilation</t>
-  </si>
-  <si>
-    <t>Assumed</t>
-  </si>
-  <si>
     <t>of</t>
   </si>
   <si>
@@ -230,20 +212,14 @@
     <t>First Monday is not included</t>
   </si>
   <si>
-    <t>Link the menu with game</t>
-  </si>
-  <si>
-    <t>Play Test &amp; Ensure game is fluid</t>
-  </si>
-  <si>
-    <t>Reserved for last minute changes</t>
+    <t>Actual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,8 +242,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,12 +301,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -348,12 +325,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -391,11 +368,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -440,31 +430,34 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -987,24 +980,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" customWidth="1"/>
     <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
     <col min="9" max="9" width="10.88671875" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" customWidth="1"/>
-    <col min="11" max="11" width="16.44140625" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" customWidth="1"/>
+    <col min="11" max="11" width="8.21875" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
     <col min="13" max="13" width="11.44140625" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" customWidth="1"/>
     <col min="15" max="15" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.88671875" customWidth="1"/>
     <col min="17" max="18" width="16.33203125" customWidth="1"/>
@@ -1354,8 +1348,8 @@
       <c r="U24" s="5"/>
     </row>
     <row r="25" spans="1:21" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="30" t="s">
-        <v>56</v>
+      <c r="A25" s="29" t="s">
+        <v>50</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>7</v>
@@ -1396,7 +1390,7 @@
       <c r="N25" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="O25" s="31" t="s">
+      <c r="O25" s="30" t="s">
         <v>10</v>
       </c>
       <c r="P25" s="5"/>
@@ -1407,7 +1401,7 @@
       <c r="U25" s="5"/>
     </row>
     <row r="26" spans="1:21" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="29" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="14"/>
@@ -1415,7 +1409,7 @@
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
-      <c r="G26" s="32" t="s">
+      <c r="G26" s="31" t="s">
         <v>37</v>
       </c>
       <c r="H26" s="13"/>
@@ -1424,12 +1418,10 @@
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
-      <c r="N26" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="O26" s="31" t="s">
+      <c r="N26" s="30" t="s">
         <v>45</v>
       </c>
+      <c r="O26" s="37"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
@@ -1438,15 +1430,15 @@
       <c r="U26" s="5"/>
     </row>
     <row r="27" spans="1:21" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="29" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="14"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
-      <c r="G27" s="32" t="s">
+      <c r="G27" s="31" t="s">
         <v>38</v>
       </c>
       <c r="H27" s="13"/>
@@ -1455,12 +1447,10 @@
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
-      <c r="N27" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="O27" s="31" t="s">
-        <v>49</v>
-      </c>
+      <c r="N27" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="O27" s="37"/>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
@@ -1469,17 +1459,15 @@
       <c r="U27" s="5"/>
     </row>
     <row r="28" spans="1:21" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="30" t="s">
-        <v>50</v>
+      <c r="A28" s="29" t="s">
+        <v>47</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="22"/>
-      <c r="D28" s="33" t="s">
-        <v>51</v>
-      </c>
+      <c r="D28" s="32"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
-      <c r="G28" s="32" t="s">
+      <c r="G28" s="31" t="s">
         <v>39</v>
       </c>
       <c r="H28" s="13"/>
@@ -1488,12 +1476,10 @@
       <c r="K28" s="13"/>
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
-      <c r="N28" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="O28" s="34" t="s">
-        <v>54</v>
-      </c>
+      <c r="N28" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="O28" s="37"/>
       <c r="P28" s="7"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
@@ -1502,7 +1488,7 @@
       <c r="U28" s="1"/>
     </row>
     <row r="29" spans="1:21" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="29" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="16"/>
@@ -1510,7 +1496,7 @@
       <c r="D29" s="26"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
-      <c r="G29" s="32" t="s">
+      <c r="G29" s="31" t="s">
         <v>43</v>
       </c>
       <c r="H29" s="13"/>
@@ -1519,12 +1505,10 @@
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
       <c r="M29" s="13"/>
-      <c r="N29" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="O29" s="34" t="s">
-        <v>49</v>
-      </c>
+      <c r="N29" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="O29" s="37"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
@@ -1533,29 +1517,27 @@
       <c r="U29" s="5"/>
     </row>
     <row r="30" spans="1:21" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="32" t="s">
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
       <c r="K30" s="13"/>
       <c r="L30" s="13"/>
       <c r="M30" s="13"/>
-      <c r="N30" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="O30" s="34" t="s">
-        <v>55</v>
-      </c>
+      <c r="N30" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="O30" s="37"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
@@ -1564,22 +1546,14 @@
       <c r="U30" s="5"/>
     </row>
     <row r="31" spans="1:21" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="30" t="s">
+      <c r="A31" s="29" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="13"/>
-      <c r="C31" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>13</v>
-      </c>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="17"/>
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
@@ -1587,12 +1561,10 @@
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
       <c r="M31" s="13"/>
-      <c r="N31" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="O31" s="34" t="s">
+      <c r="N31" s="33" t="s">
         <v>45</v>
       </c>
+      <c r="O31" s="37"/>
       <c r="P31" s="7"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
@@ -1601,27 +1573,23 @@
       <c r="U31" s="1"/>
     </row>
     <row r="32" spans="1:21" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="29" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="13"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
-      <c r="H32" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
-      <c r="N32" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="O32" s="31"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="36"/>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
@@ -1630,23 +1598,23 @@
       <c r="U32" s="5"/>
     </row>
     <row r="33" spans="1:21" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="36" t="s">
-        <v>66</v>
+      <c r="A33" s="34" t="s">
+        <v>60</v>
       </c>
       <c r="B33" s="13"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
       <c r="F33" s="13"/>
       <c r="G33" s="18"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="27"/>
       <c r="M33" s="13"/>
       <c r="N33" s="21"/>
-      <c r="O33" s="29"/>
+      <c r="O33" s="28"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
@@ -1655,7 +1623,7 @@
       <c r="U33" s="5"/>
     </row>
     <row r="34" spans="1:21" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="29" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="13"/>
@@ -1664,14 +1632,14 @@
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
       <c r="G34" s="18"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="35"/>
-      <c r="L34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
-      <c r="O34" s="31"/>
+      <c r="O34" s="30"/>
       <c r="P34" s="7"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
@@ -1687,7 +1655,7 @@
         <v>41</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D35" s="1"/>
       <c r="P35" s="5"/>
@@ -1717,7 +1685,7 @@
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1729,54 +1697,54 @@
         <v>81119746</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B39" s="23"/>
       <c r="C39" s="13">
         <v>97113472</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="24" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B40" s="26"/>
       <c r="C40" s="25" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="24" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B41" s="22"/>
       <c r="C41" s="25" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="29"/>
+        <v>54</v>
+      </c>
+      <c r="B42" s="28"/>
       <c r="C42" s="25" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1785,7 +1753,7 @@
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="25" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>